<commit_message>
program works as intended
</commit_message>
<xml_diff>
--- a/excelproject/CS1.xlsx
+++ b/excelproject/CS1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saisamarth/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saisamarth/Desktop/Projects/demo/excelproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{720B0959-0AE2-EF4E-8AA9-9DF59B06DB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E306C6D-81FD-9449-BC49-CAC67E0E702D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{ED9A240C-8F72-9A4B-A1B0-CF8FC46AAB9B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
   <si>
     <t>Servers</t>
   </si>
@@ -122,6 +122,18 @@
     <t>Cloud</t>
   </si>
   <si>
+    <t>Nilesh Patel</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>CyberSecurity</t>
+  </si>
+  <si>
     <t>Sha</t>
   </si>
   <si>
@@ -134,6 +146,15 @@
     <t>Crypto</t>
   </si>
   <si>
+    <t>Milan Patel</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
     <t>Patel</t>
   </si>
   <si>
@@ -161,9 +182,6 @@
     <t>12</t>
   </si>
   <si>
-    <t>124</t>
-  </si>
-  <si>
     <t>Kumar Singh</t>
   </si>
   <si>
@@ -173,7 +191,16 @@
     <t>103</t>
   </si>
   <si>
-    <t>CyberSecurity</t>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>284</t>
+  </si>
+  <si>
+    <t>172</t>
   </si>
 </sst>
 </file>
@@ -233,10 +260,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -536,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FC2FE6-E4DC-FE44-B2B3-F0E7F2E11640}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,32 +594,8 @@
       <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -615,32 +614,8 @@
       <c r="F2" t="s">
         <v>27</v>
       </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -648,40 +623,16 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -692,7 +643,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -700,43 +651,19 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -744,43 +671,19 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" t="s">
-        <v>37</v>
-      </c>
-      <c r="N6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -788,43 +691,19 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" t="s">
-        <v>40</v>
-      </c>
-      <c r="M7" t="s">
-        <v>41</v>
-      </c>
-      <c r="N7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -832,43 +711,19 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" t="s">
-        <v>30</v>
-      </c>
-      <c r="N8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -876,48 +731,36 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M9" t="s">
-        <v>44</v>
-      </c>
-      <c r="N9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created executable JAR file
</commit_message>
<xml_diff>
--- a/excelproject/CS1.xlsx
+++ b/excelproject/CS1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saisamarth/Desktop/Projects/demo/excelproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E306C6D-81FD-9449-BC49-CAC67E0E702D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07A5DD0-0A3E-FC41-99AC-80304C749B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{ED9A240C-8F72-9A4B-A1B0-CF8FC46AAB9B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="55">
   <si>
     <t>Servers</t>
   </si>
@@ -146,6 +146,15 @@
     <t>Crypto</t>
   </si>
   <si>
+    <t>Suraj Sharma</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
     <t>Milan Patel</t>
   </si>
   <si>
@@ -171,15 +180,6 @@
   </si>
   <si>
     <t>101</t>
-  </si>
-  <si>
-    <t>Network</t>
-  </si>
-  <si>
-    <t>Suraj Sharma</t>
-  </si>
-  <si>
-    <t>12</t>
   </si>
   <si>
     <t>Kumar Singh</t>
@@ -562,7 +562,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -635,12 +635,24 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5">
@@ -651,13 +663,13 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
         <v>35</v>
@@ -671,16 +683,16 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7">
@@ -691,10 +703,10 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
@@ -751,16 +763,16 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
         <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>